<commit_message>
changed 2 lines graphs and added in blurbs for tays, foster care, service availability, and DMHSA
</commit_message>
<xml_diff>
--- a/ShinyApp/data/smi-waitlist.xlsx
+++ b/ShinyApp/data/smi-waitlist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB0ED84-179F-5844-8F83-8D5BB77411FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B0FD54-CB85-4F42-8018-42491A1849AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15440" xr2:uid="{37288CEA-3D0D-DE41-AE9E-C0A7DE6007A5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
   <si>
     <t>SMI Status</t>
   </si>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +85,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -157,6 +170,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD2A74B-09C0-8C49-8EB9-04F67BED9BE2}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,9 +506,10 @@
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,8 +532,30 @@
         <v>1</v>
       </c>
       <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -531,8 +578,30 @@
         <v>202</v>
       </c>
       <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4">
+        <v>34</v>
+      </c>
+      <c r="K2" s="4">
+        <v>24</v>
+      </c>
+      <c r="L2" s="4">
+        <v>18</v>
+      </c>
+      <c r="M2" s="4">
+        <v>29</v>
+      </c>
+      <c r="N2" s="4">
+        <v>26</v>
+      </c>
+      <c r="O2" s="4">
+        <v>7</v>
+      </c>
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -554,8 +623,29 @@
       <c r="G3">
         <v>147</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -578,8 +668,30 @@
         <v>98</v>
       </c>
       <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="4">
+        <v>177</v>
+      </c>
+      <c r="K4" s="4">
+        <v>193</v>
+      </c>
+      <c r="L4" s="4">
+        <v>138</v>
+      </c>
+      <c r="M4" s="4">
+        <v>13</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -602,148 +714,471 @@
         <v>447</v>
       </c>
       <c r="H5" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="I5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>17</v>
+      </c>
+      <c r="M5">
+        <v>20</v>
+      </c>
+      <c r="N5">
+        <v>13</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="I6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="7">
+        <v>229</v>
+      </c>
+      <c r="K6" s="7">
+        <v>237</v>
+      </c>
+      <c r="L6" s="7">
+        <v>171</v>
+      </c>
+      <c r="M6" s="7">
+        <v>67</v>
+      </c>
+      <c r="N6" s="7">
+        <v>43</v>
+      </c>
+      <c r="O6" s="7">
+        <v>19</v>
+      </c>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>379</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2016</v>
+      </c>
+      <c r="K7" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2017</v>
+      </c>
+      <c r="C8" s="4">
+        <v>400</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2017</v>
+      </c>
+      <c r="K8" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2018</v>
+      </c>
+      <c r="C9" s="4">
+        <v>398</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K9" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="14">
+        <v>2019</v>
+      </c>
+      <c r="C10" s="4">
+        <v>401</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2019</v>
+      </c>
+      <c r="K10" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2020</v>
+      </c>
+      <c r="C11" s="4">
+        <v>302</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K11" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2016</v>
+      </c>
+      <c r="C12">
+        <v>165</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2016</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="14">
+        <v>2017</v>
+      </c>
+      <c r="C13">
+        <v>173</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2017</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="14">
+        <v>2018</v>
+      </c>
+      <c r="C14">
+        <v>182</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="14">
+        <v>2019</v>
+      </c>
+      <c r="C15">
+        <v>210</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2019</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2020</v>
+      </c>
+      <c r="C16">
+        <v>208</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K16">
         <v>6</v>
       </c>
-      <c r="B9" s="1">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="14">
         <v>2016</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C17" s="4">
+        <v>205</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2016</v>
+      </c>
+      <c r="K17" s="4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="14">
         <v>2017</v>
       </c>
-      <c r="D9" s="1">
+      <c r="C18" s="4">
+        <v>231</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2017</v>
+      </c>
+      <c r="K18" s="4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="14">
         <v>2018</v>
       </c>
-      <c r="E9" s="1">
+      <c r="C19" s="4">
+        <v>236</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K19" s="4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="14">
         <v>2019</v>
       </c>
-      <c r="F9" s="1">
+      <c r="C20" s="4">
+        <v>228</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2019</v>
+      </c>
+      <c r="K20" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="14">
         <v>2020</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
-        <v>34</v>
-      </c>
-      <c r="C10" s="4">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4">
-        <v>29</v>
-      </c>
-      <c r="F10" s="4">
-        <v>26</v>
-      </c>
-      <c r="G10" s="4">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11">
+      <c r="C21" s="4">
+        <v>171</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="J21" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="I22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F11">
-        <v>6</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4">
-        <v>177</v>
-      </c>
-      <c r="C12" s="4">
-        <v>193</v>
-      </c>
-      <c r="D12" s="4">
-        <v>138</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="J22" s="1">
+        <v>2016</v>
+      </c>
+      <c r="K22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="I23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="1">
+        <v>2017</v>
+      </c>
+      <c r="K23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="I24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="I25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1">
+        <v>2019</v>
+      </c>
+      <c r="K25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K26">
         <v>13</v>
       </c>
-      <c r="F12" s="4">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>20</v>
-      </c>
-      <c r="D13">
-        <v>17</v>
-      </c>
-      <c r="E13">
-        <v>20</v>
-      </c>
-      <c r="F13">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="7">
-        <v>229</v>
-      </c>
-      <c r="C14" s="7">
-        <v>237</v>
-      </c>
-      <c r="D14" s="7">
-        <v>171</v>
-      </c>
-      <c r="E14" s="7">
-        <v>67</v>
-      </c>
-      <c r="F14" s="7">
-        <v>43</v>
-      </c>
-      <c r="G14" s="7">
-        <v>19</v>
-      </c>
-      <c r="H14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>